<commit_message>
refract: ALU by using 16 & 8way chips
</commit_message>
<xml_diff>
--- a/projects/02/THINKING.xlsx
+++ b/projects/02/THINKING.xlsx
@@ -1,40 +1,71 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming\nand2tetris\projects\02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\50196\Documents\programming\nand2tetris\projects\02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EED9FB55-CE6F-4741-930F-AFD101AA69D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80DB958-143D-42E5-A836-999A7AABE74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{668D45AA-9FD7-42F2-BF42-17CA813BDD6F}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" activeTab="4" xr2:uid="{668D45AA-9FD7-42F2-BF42-17CA813BDD6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="ALU" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jq H</author>
+  </authors>
+  <commentList>
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{6B6661C6-ED33-423C-9410-C4A737AC0365}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Jq H:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+假设是相加等于零的表示法（补码），即radix complement</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="60">
   <si>
     <r>
       <t>HalfAdder</t>
@@ -537,12 +568,96 @@
     </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t>zy</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ny</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>out=</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>x=0</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>x=!x</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>y=0</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>y=!y</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>x+y|x&amp;y</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>out=!out</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>f(x, y)=</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>!x</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>!y</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>x+1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>y+1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>x-1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>y-1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>x+y</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>x-y</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>y-x</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>-x</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>-y</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -575,6 +690,21 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2180,7 +2310,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="b">
-        <f>AND(E15,G15)</f>
+        <f t="shared" ref="I15:I22" si="0">AND(E15,G15)</f>
         <v>0</v>
       </c>
       <c r="J15">
@@ -2207,15 +2337,15 @@
         <v>1</v>
       </c>
       <c r="G16" t="b">
-        <f t="shared" ref="G16:G22" si="0">AND(D16,F16)</f>
+        <f t="shared" ref="G16:G22" si="1">AND(D16,F16)</f>
         <v>0</v>
       </c>
       <c r="H16" t="b">
-        <f t="shared" ref="H16:H22" si="1">_xlfn.XOR(E16,G16)</f>
+        <f t="shared" ref="H16:H22" si="2">_xlfn.XOR(E16,G16)</f>
         <v>0</v>
       </c>
       <c r="I16" t="b">
-        <f>AND(E16,G16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J16">
@@ -2242,15 +2372,15 @@
         <v>1</v>
       </c>
       <c r="G17" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H17" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I17" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H17" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I17" t="b">
-        <f>AND(E17,G17)</f>
         <v>0</v>
       </c>
       <c r="J17">
@@ -2277,15 +2407,15 @@
         <v>1</v>
       </c>
       <c r="G18" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H18" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I18" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H18" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I18" t="b">
-        <f>AND(E18,G18)</f>
         <v>0</v>
       </c>
       <c r="J18">
@@ -2312,15 +2442,15 @@
         <v>0</v>
       </c>
       <c r="G19" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H19" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I19" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H19" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I19" t="b">
-        <f>AND(E19,G19)</f>
         <v>0</v>
       </c>
       <c r="J19">
@@ -2347,15 +2477,15 @@
         <v>1</v>
       </c>
       <c r="G20" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H20" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I20" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H20" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I20" t="b">
-        <f>AND(E20,G20)</f>
         <v>0</v>
       </c>
       <c r="J20">
@@ -2382,15 +2512,15 @@
         <v>1</v>
       </c>
       <c r="G21" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H21" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I21" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H21" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I21" t="b">
-        <f>AND(E21,G21)</f>
         <v>0</v>
       </c>
       <c r="J21">
@@ -2417,15 +2547,15 @@
         <v>1</v>
       </c>
       <c r="G22" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H22" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I22" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H22" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I22" t="b">
-        <f>AND(E22,G22)</f>
         <v>1</v>
       </c>
       <c r="J22">
@@ -2539,7 +2669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E93BC11F-06C4-40FC-8198-882139C15DC0}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E15"/>
     </sheetView>
   </sheetViews>
@@ -3254,4 +3384,341 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E4C4C07-38D4-4BE5-B39E-EBEE67FA833F}">
+  <dimension ref="B1:H20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="9.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="H19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>